<commit_message>
Updated prototype 2 and started user testing methodology
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 1/User Test Timings.xlsx
+++ b/Assignments/Assignment 1/User Test Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Uni Work\Year 4\Semester 1\KIT305 Mobile Applications and Development\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545C589B-187C-4B0E-914B-FBB8F63EAD0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E47EF4C-11A2-4DA3-8B43-5571C68B00F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31575" yWindow="5010" windowWidth="38700" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6810" yWindow="3885" windowWidth="38700" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>User 1</t>
   </si>
@@ -148,6 +148,48 @@
   </si>
   <si>
     <t>21.66s</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -171,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -179,12 +221,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F28"/>
+  <dimension ref="A2:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,23 +740,127 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+      <c r="G21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+      <c r="G23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F24" s="6"/>
+      <c r="G24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+      <c r="G25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -614,7 +868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -622,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -631,6 +885,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F19:M19"/>
+    <mergeCell ref="F20:F25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished tute 3 and did testing methodology in assignment 1
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 1/User Test Timings.xlsx
+++ b/Assignments/Assignment 1/User Test Timings.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Uni Work\Year 4\Semester 1\KIT305 Mobile Applications and Development\Assignments\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mobile Dev\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E47EF4C-11A2-4DA3-8B43-5571C68B00F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4F00D4-7812-4D12-A77F-3AEDAF082184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="3885" windowWidth="38700" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>User 1</t>
   </si>
@@ -63,21 +71,6 @@
     <t>User 2</t>
   </si>
   <si>
-    <t>63s</t>
-  </si>
-  <si>
-    <t>10.28s</t>
-  </si>
-  <si>
-    <t>23.48s</t>
-  </si>
-  <si>
-    <t>10.53s</t>
-  </si>
-  <si>
-    <t>38.28s</t>
-  </si>
-  <si>
     <t>Leith</t>
   </si>
   <si>
@@ -90,66 +83,9 @@
     <t>Joe</t>
   </si>
   <si>
-    <t>7.77s</t>
-  </si>
-  <si>
-    <t>30.48s</t>
-  </si>
-  <si>
-    <t>20.76s</t>
-  </si>
-  <si>
-    <t>34.04s</t>
-  </si>
-  <si>
-    <t>32.61s</t>
-  </si>
-  <si>
-    <t>88.32s</t>
-  </si>
-  <si>
-    <t>14.55s</t>
-  </si>
-  <si>
-    <t>31.04s</t>
-  </si>
-  <si>
-    <t>31.80s</t>
-  </si>
-  <si>
-    <t>26.09s</t>
-  </si>
-  <si>
-    <t>46.67s</t>
-  </si>
-  <si>
-    <t>27.70s</t>
-  </si>
-  <si>
-    <t>31.39s</t>
-  </si>
-  <si>
-    <t>30.53s</t>
-  </si>
-  <si>
     <t>DNF</t>
   </si>
   <si>
-    <t>8.45s</t>
-  </si>
-  <si>
-    <t>34.36s</t>
-  </si>
-  <si>
-    <t>20.92s</t>
-  </si>
-  <si>
-    <t>11.76s</t>
-  </si>
-  <si>
-    <t>21.66s</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -190,6 +126,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Time Users Took to Complete Tasks in Seconds</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Tasks Matrix</t>
   </si>
 </sst>
 </file>
@@ -314,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -334,6 +279,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,14 +566,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="F18" sqref="F18:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
@@ -644,105 +605,142 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+      <c r="B3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>10.28</v>
+      </c>
+      <c r="D3">
+        <v>23.48</v>
+      </c>
+      <c r="E3">
+        <v>10.53</v>
+      </c>
+      <c r="F3">
+        <v>38.28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
+      <c r="B4">
+        <v>30.48</v>
+      </c>
+      <c r="C4">
+        <v>7.77</v>
+      </c>
+      <c r="D4">
+        <v>20.76</v>
+      </c>
+      <c r="E4">
+        <v>34.04</v>
+      </c>
+      <c r="F4">
+        <v>32.61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
+      <c r="B5">
+        <v>88.32</v>
+      </c>
+      <c r="C5">
+        <v>14.55</v>
+      </c>
+      <c r="D5">
+        <v>31.04</v>
+      </c>
+      <c r="E5">
+        <v>31.8</v>
+      </c>
+      <c r="F5">
+        <v>26.09</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
+      <c r="B6">
+        <v>46.67</v>
+      </c>
+      <c r="C6">
+        <v>27.7</v>
+      </c>
+      <c r="D6">
+        <v>31.39</v>
+      </c>
+      <c r="E6">
+        <v>30.53</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
+      <c r="B7">
+        <v>34.36</v>
+      </c>
+      <c r="C7">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D7">
+        <v>11.76</v>
+      </c>
+      <c r="E7">
+        <v>20.92</v>
+      </c>
+      <c r="F7">
+        <v>21.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B3:B7)</f>
+        <v>52.56600000000001</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">AVERAGE(C3:C7)</f>
+        <v>13.75</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>23.686</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>25.564</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>29.66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F19" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -754,42 +752,42 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F20" s="5" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F21" s="6"/>
       <c r="G21" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -797,7 +795,7 @@
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F22" s="6"/>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -805,20 +803,20 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F23" s="6"/>
       <c r="G23" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="M23" s="1"/>
     </row>
@@ -831,7 +829,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -845,16 +843,16 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="1" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -865,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -873,7 +871,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -881,13 +879,15 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F19:M19"/>
     <mergeCell ref="F20:F25"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>